<commit_message>
Nearly finished refining deserializer
</commit_message>
<xml_diff>
--- a/Hotel kamers plus prices v0.2.xlsx
+++ b/Hotel kamers plus prices v0.2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ANSAID\Documents\Software track project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07B7AE75-A9EF-4F2A-B55B-59A950CEBD88}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C8ECCF-04D9-47F6-A2F3-DBC63A1F72A8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{159596B7-B20F-4450-9AD4-0E1557652CEB}"/>
   </bookViews>
@@ -80,7 +80,7 @@
     <t>2 Double bed, 1 single bed, 1 baby bed</t>
   </si>
   <si>
-    <t>2 Double bed, 4 single, 2 baby bed</t>
+    <t>2 x Double bed, 4 singles, 2 baby beds</t>
   </si>
 </sst>
 </file>
@@ -1300,7 +1300,7 @@
   <dimension ref="A1:AA20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD21"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1989,7 +1989,7 @@
   <dimension ref="A1:AC20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2832,7 +2832,7 @@
   <dimension ref="A1:U20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>